<commit_message>
Seller Check All Changes
</commit_message>
<xml_diff>
--- a/src/assets/samples/SellerProductsUpload.xlsx
+++ b/src/assets/samples/SellerProductsUpload.xlsx
@@ -10,10 +10,10 @@
   <sheets>
     <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId2"/>
   </sheets>
-  <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
+  <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
   <extLst>
     <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
-      <loext:extCalcPr stringRefSyntax="CalcA1ExcelA1"/>
+      <loext:extCalcPr stringRefSyntax="CalcA1"/>
     </ext>
   </extLst>
 </workbook>
@@ -89,13 +89,11 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="6">
-    <font>
-      <sz val="10"/>
-      <color rgb="FF000000"/>
-      <name val="Arial"/>
-      <family val="0"/>
-      <charset val="1"/>
+  <fonts count="5">
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="10"/>
@@ -118,26 +116,13 @@
       <family val="0"/>
       <charset val="1"/>
     </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF111111"/>
-      <name val="Arial"/>
-      <family val="0"/>
-      <charset val="1"/>
-    </font>
   </fonts>
-  <fills count="3">
+  <fills count="2">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFFF"/>
-        <bgColor rgb="FFFFFFCC"/>
-      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -174,16 +159,12 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="2">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -196,66 +177,6 @@
     <cellStyle name="Currency [0]" xfId="18" builtinId="7" customBuiltin="false"/>
     <cellStyle name="Percent" xfId="19" builtinId="5" customBuiltin="false"/>
   </cellStyles>
-  <colors>
-    <indexedColors>
-      <rgbColor rgb="FF000000"/>
-      <rgbColor rgb="FFFFFFFF"/>
-      <rgbColor rgb="FFFF0000"/>
-      <rgbColor rgb="FF00FF00"/>
-      <rgbColor rgb="FF0000FF"/>
-      <rgbColor rgb="FFFFFF00"/>
-      <rgbColor rgb="FFFF00FF"/>
-      <rgbColor rgb="FF00FFFF"/>
-      <rgbColor rgb="FF800000"/>
-      <rgbColor rgb="FF008000"/>
-      <rgbColor rgb="FF000080"/>
-      <rgbColor rgb="FF808000"/>
-      <rgbColor rgb="FF800080"/>
-      <rgbColor rgb="FF008080"/>
-      <rgbColor rgb="FFC0C0C0"/>
-      <rgbColor rgb="FF808080"/>
-      <rgbColor rgb="FF9999FF"/>
-      <rgbColor rgb="FF993366"/>
-      <rgbColor rgb="FFFFFFCC"/>
-      <rgbColor rgb="FFCCFFFF"/>
-      <rgbColor rgb="FF660066"/>
-      <rgbColor rgb="FFFF8080"/>
-      <rgbColor rgb="FF0066CC"/>
-      <rgbColor rgb="FFCCCCFF"/>
-      <rgbColor rgb="FF000080"/>
-      <rgbColor rgb="FFFF00FF"/>
-      <rgbColor rgb="FFFFFF00"/>
-      <rgbColor rgb="FF00FFFF"/>
-      <rgbColor rgb="FF800080"/>
-      <rgbColor rgb="FF800000"/>
-      <rgbColor rgb="FF008080"/>
-      <rgbColor rgb="FF0000FF"/>
-      <rgbColor rgb="FF00CCFF"/>
-      <rgbColor rgb="FFCCFFFF"/>
-      <rgbColor rgb="FFCCFFCC"/>
-      <rgbColor rgb="FFFFFF99"/>
-      <rgbColor rgb="FF99CCFF"/>
-      <rgbColor rgb="FFFF99CC"/>
-      <rgbColor rgb="FFCC99FF"/>
-      <rgbColor rgb="FFFFCC99"/>
-      <rgbColor rgb="FF3366FF"/>
-      <rgbColor rgb="FF33CCCC"/>
-      <rgbColor rgb="FF99CC00"/>
-      <rgbColor rgb="FFFFCC00"/>
-      <rgbColor rgb="FFFF9900"/>
-      <rgbColor rgb="FFFF6600"/>
-      <rgbColor rgb="FF666699"/>
-      <rgbColor rgb="FF969696"/>
-      <rgbColor rgb="FF003366"/>
-      <rgbColor rgb="FF339966"/>
-      <rgbColor rgb="FF111111"/>
-      <rgbColor rgb="FF333300"/>
-      <rgbColor rgb="FF993300"/>
-      <rgbColor rgb="FF993366"/>
-      <rgbColor rgb="FF333399"/>
-      <rgbColor rgb="FF333333"/>
-    </indexedColors>
-  </colors>
 </styleSheet>
 </file>
 
@@ -264,18 +185,15 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:X1048576"/>
+  <dimension ref="A1:X1"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B1" activeCellId="0" sqref="B1"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="1:1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="14.29"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="2" style="0" width="14.43"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="68.43"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="7" style="0" width="14.43"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="1" style="0" width="11.52"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -344,40 +262,13 @@
       <c r="W1" s="1"/>
       <c r="X1" s="1"/>
     </row>
-    <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="1"/>
-      <c r="B2" s="1"/>
-      <c r="C2" s="2"/>
-      <c r="D2" s="2"/>
-      <c r="E2" s="1"/>
-      <c r="F2" s="1"/>
-      <c r="G2" s="1"/>
-      <c r="H2" s="1"/>
-      <c r="I2" s="1"/>
-      <c r="J2" s="1"/>
-      <c r="K2" s="1"/>
-      <c r="L2" s="1"/>
-      <c r="M2" s="1"/>
-      <c r="N2" s="1"/>
-      <c r="O2" s="1"/>
-      <c r="P2" s="1"/>
-      <c r="Q2" s="1"/>
-      <c r="R2" s="1"/>
-      <c r="S2" s="1"/>
-      <c r="T2" s="1"/>
-      <c r="U2" s="1"/>
-      <c r="V2" s="1"/>
-      <c r="W2" s="1"/>
-      <c r="X2" s="1"/>
-    </row>
-    <row r="1048576" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.747916666666667" right="0.747916666666667" top="0.984027777777778" bottom="0.984027777777778" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader/>
-    <oddFooter/>
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
   </headerFooter>
 </worksheet>
 </file>
</xml_diff>